<commit_message>
Added SQL server connectionstring
</commit_message>
<xml_diff>
--- a/data_template.xlsx
+++ b/data_template.xlsx
@@ -20,9 +20,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="100">
   <si>
-    <t>Medve dobozos natúr 140g</t>
-  </si>
-  <si>
     <t>Medve</t>
   </si>
   <si>
@@ -32,84 +29,21 @@
     <t>Répcelak</t>
   </si>
   <si>
-    <t>Medve dobozos szalámis 140g</t>
-  </si>
-  <si>
-    <t>Medve dobozos sonkás 140g</t>
-  </si>
-  <si>
-    <t>Medve dobozos zöldfűszseres 140g</t>
-  </si>
-  <si>
-    <t>Medve dobozos csípőspaprikás 140g</t>
-  </si>
-  <si>
-    <t>Medve dobozos kolbászos 140g</t>
-  </si>
-  <si>
     <t>Medve dobozos light 140g</t>
   </si>
   <si>
-    <t>Medve dobozos laktózmentes 140g</t>
-  </si>
-  <si>
     <t>Medve dobozos mix 140g</t>
   </si>
   <si>
-    <t>Medve dobozos fokhagymás-zöldfűszeres 140g</t>
-  </si>
-  <si>
-    <t>Medve dobozos natúr 200g</t>
-  </si>
-  <si>
     <t>kördobozos 200g</t>
   </si>
   <si>
-    <t>Medve dobozos szalámis 200g</t>
-  </si>
-  <si>
-    <t>Medve dobozos sonkás 200g</t>
-  </si>
-  <si>
-    <t>Medve dobozos zöldfűszeres 200g</t>
-  </si>
-  <si>
-    <t>Medve dobozos csípős 200g</t>
-  </si>
-  <si>
-    <t>Medve dobozos kolbászos 200g</t>
-  </si>
-  <si>
-    <t>Medve dobozos natúr 280g</t>
-  </si>
-  <si>
     <t>kördobozos 280g</t>
   </si>
   <si>
-    <t>Medve dobozos szalámis 280g</t>
-  </si>
-  <si>
-    <t>Medve dobozos sonkás 280g</t>
-  </si>
-  <si>
-    <t>Medve dobozos csípős 280g</t>
-  </si>
-  <si>
-    <t>Medve tömlős natúr 100g</t>
-  </si>
-  <si>
     <t>tömlős 100g</t>
   </si>
   <si>
-    <t>Medve tömlős csípős 100g</t>
-  </si>
-  <si>
-    <t>Medve tömlős zöldfűszeres 100g</t>
-  </si>
-  <si>
-    <t>Medve tömlős tejszínes 100g</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -197,127 +131,193 @@
     <t>szeletelt</t>
   </si>
   <si>
-    <t>EXPORT Medve dobozos natúr 140g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos szalámis 140g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos sonkás 140g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos zöldfűszseres 140g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos csípőspaprikás 140g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos kolbászos 140g</t>
-  </si>
-  <si>
     <t>EXPORT Medve dobozos light 140g</t>
   </si>
   <si>
-    <t>EXPORT Medve dobozos laktózmentes 140g</t>
-  </si>
-  <si>
     <t>EXPORT Medve dobozos mix 140g</t>
   </si>
   <si>
-    <t>EXPORT Medve dobozos fokhagymás-zöldfűszeres 140g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos natúr 200g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos szalámis 200g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos sonkás 200g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos zöldfűszeres 200g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos csípős 200g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos kolbászos 200g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos natúr 280g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos szalámis 280g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos sonkás 280g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve dobozos csípős 280g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve tömlős natúr 100g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve tömlős csípős 100g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve tömlős zöldfűszeres 100g</t>
-  </si>
-  <si>
-    <t>EXPORT Medve tömlős tejszínes 100g</t>
-  </si>
-  <si>
-    <t>Karaván natúr tömb 1,2kg</t>
-  </si>
-  <si>
-    <t>Karaván fokhagymás tömb 1,2kg</t>
-  </si>
-  <si>
-    <t>Karaván sonkás tömb 1,2kg</t>
-  </si>
-  <si>
-    <t>Karaván nutellás tömb 1,2kg</t>
-  </si>
-  <si>
     <t>Private label</t>
   </si>
   <si>
-    <t>Karaván natúr tömb 2,5kg</t>
-  </si>
-  <si>
-    <t>Karaván fokhagymás tömb 2,5kg</t>
-  </si>
-  <si>
-    <t>Karaván sonkás tömb 2,5kg</t>
-  </si>
-  <si>
-    <t>Karaván natúr kördobozos 140g</t>
-  </si>
-  <si>
-    <t>Karaván fokhagymás kördobozos 140g</t>
-  </si>
-  <si>
-    <t>Karaván sonkás kördobozos 140g</t>
-  </si>
-  <si>
-    <t>Karaván natúr tömlős 100g</t>
-  </si>
-  <si>
-    <t>Karaván fokhagymás tömlős 100g</t>
-  </si>
-  <si>
-    <t>Karaván sonkás tömlős 100g</t>
-  </si>
-  <si>
-    <t>Pannónia tömb 1,2kg</t>
-  </si>
-  <si>
-    <t>Pannónia light tömb 1,2kg</t>
-  </si>
-  <si>
-    <t>Pannónia bársony tömb 1,2kg</t>
+    <t>Medve dobozos natur 140g</t>
+  </si>
+  <si>
+    <t>Medve dobozos natur 200g</t>
+  </si>
+  <si>
+    <t>Medve dobozos natur 280g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos natur 140g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos natur 200g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos natur 280g</t>
+  </si>
+  <si>
+    <t>Medve dobozos szalamis 140g</t>
+  </si>
+  <si>
+    <t>Medve dobozos sonkas 140g</t>
+  </si>
+  <si>
+    <t>Medve dobozos kolbaszos 140g</t>
+  </si>
+  <si>
+    <t>Medve dobozos szalamis 200g</t>
+  </si>
+  <si>
+    <t>Medve dobozos sonkas 200g</t>
+  </si>
+  <si>
+    <t>Medve dobozos kolbaszos 200g</t>
+  </si>
+  <si>
+    <t>Medve dobozos szalamis 280g</t>
+  </si>
+  <si>
+    <t>Medve dobozos sonkas 280g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos szalamis 140g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos sonkas 140g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos kolbaszos 140g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos szalamis 200g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos sonkas 200g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos kolbaszos 200g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos szalamis 280g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos sonkas 280g</t>
+  </si>
+  <si>
+    <t>Karavan natur tomb 1,2kg</t>
+  </si>
+  <si>
+    <t>Karavan fokhagymas tomb 1,2kg</t>
+  </si>
+  <si>
+    <t>Karavan sonkas tomb 1,2kg</t>
+  </si>
+  <si>
+    <t>Karavan nutellas tomb 1,2kg</t>
+  </si>
+  <si>
+    <t>Karavan natur tomb 2,5kg</t>
+  </si>
+  <si>
+    <t>Karavan fokhagymas tomb 2,5kg</t>
+  </si>
+  <si>
+    <t>Karavan sonkas tomb 2,5kg</t>
+  </si>
+  <si>
+    <t>Karavan natur kordobozos 140g</t>
+  </si>
+  <si>
+    <t>Karavan fokhagymas kordobozos 140g</t>
+  </si>
+  <si>
+    <t>Karavan sonkas kordobozos 140g</t>
+  </si>
+  <si>
+    <t>Pannonia tomb 1,2kg</t>
+  </si>
+  <si>
+    <t>Pannonia light tomb 1,2kg</t>
+  </si>
+  <si>
+    <t>Pannonia barsony tomb 1,2kg</t>
+  </si>
+  <si>
+    <t>Medve dobozos zoldfuszseres 140g</t>
+  </si>
+  <si>
+    <t>Medve dobozos fokhagymas-zoldfuszeres 140g</t>
+  </si>
+  <si>
+    <t>Medve dobozos zoldfuszeres 200g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos zoldfuszseres 140g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos fokhagymas-zoldfuszeres 140g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos zoldfuszeres 200g</t>
+  </si>
+  <si>
+    <t>Medve tomlos natur 100g</t>
+  </si>
+  <si>
+    <t>Medve tomlos zoldfuszeres 100g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve tomlos natur 100g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve tomlos zoldfuszeres 100g</t>
+  </si>
+  <si>
+    <t>Karavan natur tomlos 100g</t>
+  </si>
+  <si>
+    <t>Karavan fokhagymas tomlos 100g</t>
+  </si>
+  <si>
+    <t>Karavan sonkas tomlos 100g</t>
+  </si>
+  <si>
+    <t>Medve dobozos csipospaprikas 140g</t>
+  </si>
+  <si>
+    <t>Medve dobozos csipos 200g</t>
+  </si>
+  <si>
+    <t>Medve dobozos csipos 280g</t>
+  </si>
+  <si>
+    <t>Medve tomlos csipos 100g</t>
+  </si>
+  <si>
+    <t>Medve tomlos tejszines 100g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos csipospaprikas 140g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos csipos 200g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos csipos 280g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve tomlos csipos 100g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve tomlos tejszines 100g</t>
+  </si>
+  <si>
+    <t>Medve dobozos laktozmentes 140g</t>
+  </si>
+  <si>
+    <t>EXPORT Medve dobozos laktozmentes 140g</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1146,7 @@
   <dimension ref="A1:O193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1157,49 +1157,49 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="J1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="L1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="N1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="O1" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -1207,7 +1207,7 @@
         <v>1000</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1248,7 +1248,7 @@
         <v>1000</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1289,7 +1289,7 @@
         <v>1000</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1330,7 +1330,7 @@
         <v>1001</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1371,7 +1371,7 @@
         <v>1001</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1412,7 +1412,7 @@
         <v>1001</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1453,7 +1453,7 @@
         <v>1002</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1494,7 +1494,7 @@
         <v>1002</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1535,7 +1535,7 @@
         <v>1002</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1576,7 +1576,7 @@
         <v>1003</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1617,7 +1617,7 @@
         <v>1003</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1658,7 +1658,7 @@
         <v>1003</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1699,7 +1699,7 @@
         <v>1004</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1740,7 +1740,7 @@
         <v>1004</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1781,7 +1781,7 @@
         <v>1004</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1822,7 +1822,7 @@
         <v>1005</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1863,7 +1863,7 @@
         <v>1005</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1904,7 +1904,7 @@
         <v>1005</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1945,7 +1945,7 @@
         <v>1006</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1986,7 +1986,7 @@
         <v>1006</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2027,7 +2027,7 @@
         <v>1006</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2068,7 +2068,7 @@
         <v>1007</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2109,7 +2109,7 @@
         <v>1007</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -2150,7 +2150,7 @@
         <v>1007</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -2191,7 +2191,7 @@
         <v>1008</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2232,7 +2232,7 @@
         <v>1008</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2273,7 +2273,7 @@
         <v>1008</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -2314,7 +2314,7 @@
         <v>1009</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -2355,7 +2355,7 @@
         <v>1009</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -2396,7 +2396,7 @@
         <v>1009</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -2437,7 +2437,7 @@
         <v>1010</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -2478,7 +2478,7 @@
         <v>1010</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2519,7 +2519,7 @@
         <v>1010</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -2560,7 +2560,7 @@
         <v>1011</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -2601,7 +2601,7 @@
         <v>1011</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -2642,7 +2642,7 @@
         <v>1011</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -2683,7 +2683,7 @@
         <v>1012</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -2724,7 +2724,7 @@
         <v>1012</v>
       </c>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -2765,7 +2765,7 @@
         <v>1012</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -2806,7 +2806,7 @@
         <v>1013</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2847,7 +2847,7 @@
         <v>1013</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -2888,7 +2888,7 @@
         <v>1013</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2929,7 +2929,7 @@
         <v>1014</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2970,7 +2970,7 @@
         <v>1014</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3011,7 +3011,7 @@
         <v>1014</v>
       </c>
       <c r="C46" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -3052,7 +3052,7 @@
         <v>1015</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -3093,7 +3093,7 @@
         <v>1015</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -3134,7 +3134,7 @@
         <v>1015</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -3175,7 +3175,7 @@
         <v>1020</v>
       </c>
       <c r="C50" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -3216,7 +3216,7 @@
         <v>1020</v>
       </c>
       <c r="C51" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3257,7 +3257,7 @@
         <v>1020</v>
       </c>
       <c r="C52" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3298,7 +3298,7 @@
         <v>1021</v>
       </c>
       <c r="C53" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -3339,7 +3339,7 @@
         <v>1021</v>
       </c>
       <c r="C54" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -3380,7 +3380,7 @@
         <v>1021</v>
       </c>
       <c r="C55" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -3421,7 +3421,7 @@
         <v>1022</v>
       </c>
       <c r="C56" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -3462,7 +3462,7 @@
         <v>1022</v>
       </c>
       <c r="C57" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -3503,7 +3503,7 @@
         <v>1022</v>
       </c>
       <c r="C58" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -3544,7 +3544,7 @@
         <v>1023</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -3585,7 +3585,7 @@
         <v>1023</v>
       </c>
       <c r="C60" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -3626,7 +3626,7 @@
         <v>1023</v>
       </c>
       <c r="C61" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -3667,7 +3667,7 @@
         <v>1030</v>
       </c>
       <c r="C62" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -3708,7 +3708,7 @@
         <v>1030</v>
       </c>
       <c r="C63" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -3749,7 +3749,7 @@
         <v>1030</v>
       </c>
       <c r="C64" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -3790,7 +3790,7 @@
         <v>1031</v>
       </c>
       <c r="C65" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -3831,7 +3831,7 @@
         <v>1031</v>
       </c>
       <c r="C66" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -3872,7 +3872,7 @@
         <v>1031</v>
       </c>
       <c r="C67" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -3913,7 +3913,7 @@
         <v>1032</v>
       </c>
       <c r="C68" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -3954,7 +3954,7 @@
         <v>1032</v>
       </c>
       <c r="C69" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -3995,7 +3995,7 @@
         <v>1032</v>
       </c>
       <c r="C70" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -4036,7 +4036,7 @@
         <v>1033</v>
       </c>
       <c r="C71" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -4077,7 +4077,7 @@
         <v>1033</v>
       </c>
       <c r="C72" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -4118,7 +4118,7 @@
         <v>1033</v>
       </c>
       <c r="C73" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -4159,7 +4159,7 @@
         <v>9000</v>
       </c>
       <c r="C74" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -4200,7 +4200,7 @@
         <v>9000</v>
       </c>
       <c r="C75" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -4241,7 +4241,7 @@
         <v>9000</v>
       </c>
       <c r="C76" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -4282,7 +4282,7 @@
         <v>9001</v>
       </c>
       <c r="C77" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -4323,7 +4323,7 @@
         <v>9001</v>
       </c>
       <c r="C78" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -4364,7 +4364,7 @@
         <v>9001</v>
       </c>
       <c r="C79" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -4405,7 +4405,7 @@
         <v>9002</v>
       </c>
       <c r="C80" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -4446,7 +4446,7 @@
         <v>9002</v>
       </c>
       <c r="C81" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -4487,7 +4487,7 @@
         <v>9002</v>
       </c>
       <c r="C82" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -4528,7 +4528,7 @@
         <v>9003</v>
       </c>
       <c r="C83" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -4569,7 +4569,7 @@
         <v>9003</v>
       </c>
       <c r="C84" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -4610,7 +4610,7 @@
         <v>9003</v>
       </c>
       <c r="C85" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -4651,7 +4651,7 @@
         <v>9004</v>
       </c>
       <c r="C86" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -4692,7 +4692,7 @@
         <v>9004</v>
       </c>
       <c r="C87" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -4733,7 +4733,7 @@
         <v>9004</v>
       </c>
       <c r="C88" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="D88">
         <v>1</v>
@@ -4774,7 +4774,7 @@
         <v>9005</v>
       </c>
       <c r="C89" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -4815,7 +4815,7 @@
         <v>9005</v>
       </c>
       <c r="C90" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -4856,7 +4856,7 @@
         <v>9005</v>
       </c>
       <c r="C91" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -4897,7 +4897,7 @@
         <v>9006</v>
       </c>
       <c r="C92" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="D92">
         <v>1</v>
@@ -4938,7 +4938,7 @@
         <v>9006</v>
       </c>
       <c r="C93" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -4979,7 +4979,7 @@
         <v>9006</v>
       </c>
       <c r="C94" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -5020,7 +5020,7 @@
         <v>9007</v>
       </c>
       <c r="C95" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -5061,7 +5061,7 @@
         <v>9007</v>
       </c>
       <c r="C96" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -5102,7 +5102,7 @@
         <v>9007</v>
       </c>
       <c r="C97" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -5143,7 +5143,7 @@
         <v>9008</v>
       </c>
       <c r="C98" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -5184,7 +5184,7 @@
         <v>9008</v>
       </c>
       <c r="C99" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -5225,7 +5225,7 @@
         <v>9008</v>
       </c>
       <c r="C100" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -5266,7 +5266,7 @@
         <v>9009</v>
       </c>
       <c r="C101" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -5307,7 +5307,7 @@
         <v>9009</v>
       </c>
       <c r="C102" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D102">
         <v>1</v>
@@ -5348,7 +5348,7 @@
         <v>9009</v>
       </c>
       <c r="C103" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -5389,7 +5389,7 @@
         <v>9010</v>
       </c>
       <c r="C104" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -5430,7 +5430,7 @@
         <v>9010</v>
       </c>
       <c r="C105" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -5471,7 +5471,7 @@
         <v>9010</v>
       </c>
       <c r="C106" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -5512,7 +5512,7 @@
         <v>9011</v>
       </c>
       <c r="C107" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D107">
         <v>1</v>
@@ -5553,7 +5553,7 @@
         <v>9011</v>
       </c>
       <c r="C108" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -5594,7 +5594,7 @@
         <v>9011</v>
       </c>
       <c r="C109" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -5635,7 +5635,7 @@
         <v>9012</v>
       </c>
       <c r="C110" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -5676,7 +5676,7 @@
         <v>9012</v>
       </c>
       <c r="C111" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -5717,7 +5717,7 @@
         <v>9012</v>
       </c>
       <c r="C112" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D112">
         <v>1</v>
@@ -5758,7 +5758,7 @@
         <v>9013</v>
       </c>
       <c r="C113" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D113">
         <v>1</v>
@@ -5799,7 +5799,7 @@
         <v>9013</v>
       </c>
       <c r="C114" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D114">
         <v>1</v>
@@ -5840,7 +5840,7 @@
         <v>9013</v>
       </c>
       <c r="C115" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -5881,7 +5881,7 @@
         <v>9014</v>
       </c>
       <c r="C116" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -5922,7 +5922,7 @@
         <v>9014</v>
       </c>
       <c r="C117" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="D117">
         <v>1</v>
@@ -5963,7 +5963,7 @@
         <v>9014</v>
       </c>
       <c r="C118" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="D118">
         <v>1</v>
@@ -6004,7 +6004,7 @@
         <v>9015</v>
       </c>
       <c r="C119" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D119">
         <v>1</v>
@@ -6045,7 +6045,7 @@
         <v>9015</v>
       </c>
       <c r="C120" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D120">
         <v>1</v>
@@ -6086,7 +6086,7 @@
         <v>9015</v>
       </c>
       <c r="C121" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D121">
         <v>1</v>
@@ -6127,7 +6127,7 @@
         <v>9020</v>
       </c>
       <c r="C122" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="D122">
         <v>1</v>
@@ -6168,7 +6168,7 @@
         <v>9020</v>
       </c>
       <c r="C123" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="D123">
         <v>1</v>
@@ -6209,7 +6209,7 @@
         <v>9020</v>
       </c>
       <c r="C124" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="D124">
         <v>1</v>
@@ -6250,7 +6250,7 @@
         <v>9021</v>
       </c>
       <c r="C125" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D125">
         <v>1</v>
@@ -6291,7 +6291,7 @@
         <v>9021</v>
       </c>
       <c r="C126" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D126">
         <v>1</v>
@@ -6332,7 +6332,7 @@
         <v>9021</v>
       </c>
       <c r="C127" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D127">
         <v>1</v>
@@ -6373,7 +6373,7 @@
         <v>9022</v>
       </c>
       <c r="C128" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D128">
         <v>1</v>
@@ -6414,7 +6414,7 @@
         <v>9022</v>
       </c>
       <c r="C129" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D129">
         <v>1</v>
@@ -6455,7 +6455,7 @@
         <v>9022</v>
       </c>
       <c r="C130" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D130">
         <v>1</v>
@@ -6496,7 +6496,7 @@
         <v>9023</v>
       </c>
       <c r="C131" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="D131">
         <v>1</v>
@@ -6537,7 +6537,7 @@
         <v>9023</v>
       </c>
       <c r="C132" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="D132">
         <v>1</v>
@@ -6578,7 +6578,7 @@
         <v>9023</v>
       </c>
       <c r="C133" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="D133">
         <v>1</v>
@@ -6619,7 +6619,7 @@
         <v>9030</v>
       </c>
       <c r="C134" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D134">
         <v>1</v>
@@ -6660,7 +6660,7 @@
         <v>9030</v>
       </c>
       <c r="C135" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D135">
         <v>1</v>
@@ -6701,7 +6701,7 @@
         <v>9030</v>
       </c>
       <c r="C136" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D136">
         <v>1</v>
@@ -6742,7 +6742,7 @@
         <v>9031</v>
       </c>
       <c r="C137" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D137">
         <v>1</v>
@@ -6783,7 +6783,7 @@
         <v>9031</v>
       </c>
       <c r="C138" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D138">
         <v>1</v>
@@ -6824,7 +6824,7 @@
         <v>9031</v>
       </c>
       <c r="C139" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D139">
         <v>1</v>
@@ -6865,7 +6865,7 @@
         <v>9032</v>
       </c>
       <c r="C140" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D140">
         <v>1</v>
@@ -6906,7 +6906,7 @@
         <v>9032</v>
       </c>
       <c r="C141" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D141">
         <v>1</v>
@@ -6947,7 +6947,7 @@
         <v>9032</v>
       </c>
       <c r="C142" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D142">
         <v>1</v>
@@ -6988,7 +6988,7 @@
         <v>9033</v>
       </c>
       <c r="C143" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="D143">
         <v>1</v>
@@ -7029,7 +7029,7 @@
         <v>9033</v>
       </c>
       <c r="C144" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="D144">
         <v>1</v>
@@ -7070,7 +7070,7 @@
         <v>9033</v>
       </c>
       <c r="C145" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="D145">
         <v>1</v>
@@ -7111,7 +7111,7 @@
         <v>2000</v>
       </c>
       <c r="C146" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D146">
         <v>2</v>
@@ -7152,7 +7152,7 @@
         <v>2000</v>
       </c>
       <c r="C147" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D147">
         <v>2</v>
@@ -7193,7 +7193,7 @@
         <v>2000</v>
       </c>
       <c r="C148" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D148">
         <v>2</v>
@@ -7234,7 +7234,7 @@
         <v>2001</v>
       </c>
       <c r="C149" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D149">
         <v>2</v>
@@ -7275,7 +7275,7 @@
         <v>2001</v>
       </c>
       <c r="C150" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D150">
         <v>2</v>
@@ -7316,7 +7316,7 @@
         <v>2001</v>
       </c>
       <c r="C151" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D151">
         <v>2</v>
@@ -7357,7 +7357,7 @@
         <v>2002</v>
       </c>
       <c r="C152" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D152">
         <v>2</v>
@@ -7398,7 +7398,7 @@
         <v>2002</v>
       </c>
       <c r="C153" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D153">
         <v>2</v>
@@ -7439,7 +7439,7 @@
         <v>2002</v>
       </c>
       <c r="C154" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D154">
         <v>2</v>
@@ -7480,7 +7480,7 @@
         <v>2003</v>
       </c>
       <c r="C155" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D155">
         <v>2</v>
@@ -7521,7 +7521,7 @@
         <v>2003</v>
       </c>
       <c r="C156" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D156">
         <v>2</v>
@@ -7562,7 +7562,7 @@
         <v>2003</v>
       </c>
       <c r="C157" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D157">
         <v>2</v>
@@ -7603,7 +7603,7 @@
         <v>2004</v>
       </c>
       <c r="C158" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="D158">
         <v>2</v>
@@ -7644,7 +7644,7 @@
         <v>2004</v>
       </c>
       <c r="C159" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="D159">
         <v>2</v>
@@ -7685,7 +7685,7 @@
         <v>2004</v>
       </c>
       <c r="C160" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="D160">
         <v>2</v>
@@ -7726,7 +7726,7 @@
         <v>2005</v>
       </c>
       <c r="C161" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D161">
         <v>2</v>
@@ -7767,7 +7767,7 @@
         <v>2005</v>
       </c>
       <c r="C162" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D162">
         <v>2</v>
@@ -7808,7 +7808,7 @@
         <v>2005</v>
       </c>
       <c r="C163" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="D163">
         <v>2</v>
@@ -7849,7 +7849,7 @@
         <v>2006</v>
       </c>
       <c r="C164" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="D164">
         <v>2</v>
@@ -7890,7 +7890,7 @@
         <v>2006</v>
       </c>
       <c r="C165" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="D165">
         <v>2</v>
@@ -7931,7 +7931,7 @@
         <v>2006</v>
       </c>
       <c r="C166" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="D166">
         <v>2</v>
@@ -7972,7 +7972,7 @@
         <v>2007</v>
       </c>
       <c r="C167" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="D167">
         <v>2</v>
@@ -8013,7 +8013,7 @@
         <v>2007</v>
       </c>
       <c r="C168" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="D168">
         <v>2</v>
@@ -8054,7 +8054,7 @@
         <v>2007</v>
       </c>
       <c r="C169" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="D169">
         <v>2</v>
@@ -8095,7 +8095,7 @@
         <v>2008</v>
       </c>
       <c r="C170" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="D170">
         <v>2</v>
@@ -8136,7 +8136,7 @@
         <v>2008</v>
       </c>
       <c r="C171" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="D171">
         <v>2</v>
@@ -8177,7 +8177,7 @@
         <v>2008</v>
       </c>
       <c r="C172" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="D172">
         <v>2</v>
@@ -8218,7 +8218,7 @@
         <v>2009</v>
       </c>
       <c r="C173" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="D173">
         <v>2</v>
@@ -8259,7 +8259,7 @@
         <v>2009</v>
       </c>
       <c r="C174" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="D174">
         <v>2</v>
@@ -8300,7 +8300,7 @@
         <v>2009</v>
       </c>
       <c r="C175" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="D175">
         <v>2</v>
@@ -8341,7 +8341,7 @@
         <v>2010</v>
       </c>
       <c r="C176" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D176">
         <v>2</v>
@@ -8382,7 +8382,7 @@
         <v>2010</v>
       </c>
       <c r="C177" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D177">
         <v>2</v>
@@ -8423,7 +8423,7 @@
         <v>2010</v>
       </c>
       <c r="C178" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D178">
         <v>2</v>
@@ -8464,7 +8464,7 @@
         <v>2010</v>
       </c>
       <c r="C179" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D179">
         <v>2</v>
@@ -8505,7 +8505,7 @@
         <v>2011</v>
       </c>
       <c r="C180" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D180">
         <v>2</v>
@@ -8546,7 +8546,7 @@
         <v>2011</v>
       </c>
       <c r="C181" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D181">
         <v>2</v>
@@ -8587,7 +8587,7 @@
         <v>2010</v>
       </c>
       <c r="C182" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D182">
         <v>2</v>
@@ -8628,7 +8628,7 @@
         <v>2012</v>
       </c>
       <c r="C183" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D183">
         <v>2</v>
@@ -8669,7 +8669,7 @@
         <v>2012</v>
       </c>
       <c r="C184" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D184">
         <v>2</v>
@@ -8710,7 +8710,7 @@
         <v>3000</v>
       </c>
       <c r="C185" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D185">
         <v>3</v>
@@ -8751,7 +8751,7 @@
         <v>3000</v>
       </c>
       <c r="C186" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D186">
         <v>3</v>
@@ -8792,7 +8792,7 @@
         <v>3000</v>
       </c>
       <c r="C187" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D187">
         <v>3</v>
@@ -8833,7 +8833,7 @@
         <v>3001</v>
       </c>
       <c r="C188" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="D188">
         <v>3</v>
@@ -8874,7 +8874,7 @@
         <v>3001</v>
       </c>
       <c r="C189" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="D189">
         <v>3</v>
@@ -8915,7 +8915,7 @@
         <v>3001</v>
       </c>
       <c r="C190" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="D190">
         <v>3</v>
@@ -8956,7 +8956,7 @@
         <v>3002</v>
       </c>
       <c r="C191" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="D191">
         <v>3</v>
@@ -8997,7 +8997,7 @@
         <v>3002</v>
       </c>
       <c r="C192" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="D192">
         <v>3</v>
@@ -9038,7 +9038,7 @@
         <v>3002</v>
       </c>
       <c r="C193" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="D193">
         <v>3</v>
@@ -9095,15 +9095,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -9111,7 +9111,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -9119,7 +9119,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -9127,15 +9127,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -9143,7 +9143,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -9151,7 +9151,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -9159,7 +9159,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -9167,7 +9167,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -9175,7 +9175,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -9183,7 +9183,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>7</v>
@@ -9191,7 +9191,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -9199,15 +9199,15 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -9215,7 +9215,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -9223,7 +9223,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -9231,15 +9231,15 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -9247,7 +9247,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -9255,7 +9255,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -9263,15 +9263,15 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -9279,7 +9279,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -9287,7 +9287,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>3</v>

</xml_diff>